<commit_message>
prepare tony's dataset, and setup intelligent ocr
</commit_message>
<xml_diff>
--- a/Assets/database.xlsx
+++ b/Assets/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mouya\Documents\UiPath\InvoiceProcessing\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF50285-509E-4C77-8081-5AB4059269AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B15DD06-110C-45A3-8EF9-C8F647BED13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -348,7 +348,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
@@ -364,6 +364,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>